<commit_message>
fixed preflop auto-ai case errors
</commit_message>
<xml_diff>
--- a/test/evdiffv2.xlsx
+++ b/test/evdiffv2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a89796590138a2f1/python-projects/pypokertools/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="8_{EE9AF03F-5CA0-4879-86AE-4AA64A52EA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A507D2C8-2A5D-4212-955E-B1F3F8555F94}"/>
+  <xr:revisionPtr revIDLastSave="212" documentId="8_{EE9AF03F-5CA0-4879-86AE-4AA64A52EA03}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{BF71D781-F687-4AC7-9F9D-FBDECC1DD037}"/>
   <bookViews>
-    <workbookView xWindow="90" yWindow="60" windowWidth="25065" windowHeight="17265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19140" yWindow="225" windowWidth="18930" windowHeight="15735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2way" sheetId="1" r:id="rId1"/>
@@ -612,7 +612,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="202">
   <si>
     <t>hand</t>
   </si>
@@ -1209,6 +1209,15 @@
   </si>
   <si>
     <t>sat16\round1\2way\hero-call-bvb.txt</t>
+  </si>
+  <si>
+    <t>6d8s</t>
+  </si>
+  <si>
+    <t>8d9d</t>
+  </si>
+  <si>
+    <t>sat16\round1\auto-ai.txt</t>
   </si>
 </sst>
 </file>
@@ -1760,118 +1769,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color rgb="FFFF0000"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FFFF0000"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thick">
-          <color rgb="FF0070C0"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF0070C0"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thick">
-          <color rgb="FF0070C0"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     </dxf>
     <dxf>
@@ -4126,6 +4023,118 @@
         </right>
       </border>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color rgb="FFFF0000"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FFFF0000"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thick">
+          <color rgb="FF0070C0"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF0070C0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thick">
+          <color rgb="FF0070C0"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -4152,47 +4161,47 @@
     <tableColumn id="22" xr3:uid="{606BE3B6-146B-4D73-A0DB-38DC0878C8F6}" name="stack"/>
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="hand"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="pWin"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="stackwin" dataDxfId="27" totalsRowDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="stackwin" dataDxfId="291" totalsRowDxfId="12"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="EQwin"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ICMwin" dataDxfId="26" totalsRowDxfId="11">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ICMwin" dataDxfId="290" totalsRowDxfId="11">
       <calculatedColumnFormula>Table2[[#This Row],[EQwin]]*$E$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Kowin" dataDxfId="25" totalsRowDxfId="10">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Kowin" dataDxfId="289" totalsRowDxfId="10">
       <calculatedColumnFormula>2*Table2[[#This Row],[stackwin]]/3000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="stacklose" dataDxfId="24" totalsRowDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="stacklose" dataDxfId="288" totalsRowDxfId="9"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="EQlose"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ICMlose" dataDxfId="23" totalsRowDxfId="8">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="ICMlose" dataDxfId="287" totalsRowDxfId="8">
       <calculatedColumnFormula>I8*$E$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Kolose" dataDxfId="22" totalsRowDxfId="7">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Kolose" dataDxfId="286" totalsRowDxfId="7">
       <calculatedColumnFormula>5*Table2[[#This Row],[stacklose]]/3000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name=" 2"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="stackfact" dataDxfId="21" totalsRowDxfId="6"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="stackfact" dataDxfId="285" totalsRowDxfId="6"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Eqfact"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="ICMFact" dataDxfId="20" totalsRowDxfId="5">
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="ICMFact" dataDxfId="284" totalsRowDxfId="5">
       <calculatedColumnFormula>N8*$E$1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="KOFact" dataDxfId="19" totalsRowDxfId="4">
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="KOFact" dataDxfId="283" totalsRowDxfId="4">
       <calculatedColumnFormula>5*Table2[[#This Row],[stackfact]]/3000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="eqdiff" dataDxfId="18">
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="eqdiff" dataDxfId="282">
       <calculatedColumnFormula>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ICMdiff" dataDxfId="17" totalsRowDxfId="3">
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="ICMdiff" dataDxfId="281" totalsRowDxfId="3">
       <calculatedColumnFormula>Table2[[#This Row],[pWin]]*Table2[[#This Row],[ICMwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[ICMlose]]-Table2[[#This Row],[ICMFact]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="KODiff" dataDxfId="16" totalsRowDxfId="2">
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="KODiff" dataDxfId="280" totalsRowDxfId="2">
       <calculatedColumnFormula>Table2[[#This Row],[Kowin]]*Table2[[#This Row],[pWin]]+Table2[[#This Row],[Kolose]]*(1-Table2[[#This Row],[pWin]])-Table2[[#This Row],[KOFact]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="KOmoneyDiff" dataDxfId="15" totalsRowDxfId="1">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="KOmoneyDiff" dataDxfId="279" totalsRowDxfId="1">
       <calculatedColumnFormula>Table2[[#This Row],[KODiff]]*bounty</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="totalDiff" dataDxfId="14" totalsRowDxfId="0">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="totalDiff" dataDxfId="278" totalsRowDxfId="0">
       <calculatedColumnFormula>Table2[[#This Row],[ICMdiff]]+Table2[[#This Row],[KOmoneyDiff]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="cEVDiff" dataDxfId="13">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="cEVDiff" dataDxfId="277">
       <calculatedColumnFormula>Table2[[#This Row],[pWin]]*Table2[[#This Row],[stackwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[stacklose]]-Table2[[#This Row],[stackfact]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4201,23 +4210,23 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="T_p4p3p1" displayName="T_p4p3p1" ref="AV15:BA21" totalsRowShown="0" tableBorderDxfId="203">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{00000000-000C-0000-FFFF-FFFF09000000}" name="T_p4p3p1" displayName="T_p4p3p1" ref="AV15:BA21" totalsRowShown="0" tableBorderDxfId="188">
   <autoFilter ref="AV15:BA21" xr:uid="{00000000-0009-0000-0100-00000B000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="players" dataDxfId="202">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0900-000001000000}" name="players" dataDxfId="187">
       <calculatedColumnFormula>COUNTIF(T_p4p3p1[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="stack" dataDxfId="201">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0900-000002000000}" name="stack" dataDxfId="186">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,uncalled+sidepot2,IF(T_init[[#This Row],[p]]=3,sidepot1,IF(T_init[[#This Row],[p]]=4,mainpot,IF(ISBLANK(T_init[[#This Row],[p]]),T_init[[#This Row],[stack]],0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0900-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="ICM" dataDxfId="200">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0900-000004000000}" name="ICM" dataDxfId="185">
       <calculatedColumnFormula>T_p4p3p1[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="KO" dataDxfId="199">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0900-000005000000}" name="KO" dataDxfId="184">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,T_p4p3p1[[#This Row],[players]]*T_p4p3p1[[#This Row],[stack]]/chips+1,T_p4p3p1[[#This Row],[players]]*T_p4p3p1[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="$stack" dataDxfId="198">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0900-000006000000}" name="$stack" dataDxfId="183">
       <calculatedColumnFormula>T_p4p3p1[[#This Row],[ICM]]+bounty*T_p4p3p1[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4226,23 +4235,23 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="T_p4p3p2" displayName="T_p4p3p2" ref="BC15:BH21" totalsRowShown="0" tableBorderDxfId="197">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{00000000-000C-0000-FFFF-FFFF0A000000}" name="T_p4p3p2" displayName="T_p4p3p2" ref="BC15:BH21" totalsRowShown="0" tableBorderDxfId="182">
   <autoFilter ref="BC15:BH21" xr:uid="{00000000-0009-0000-0100-00000C000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="players" dataDxfId="196">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0A00-000001000000}" name="players" dataDxfId="181">
       <calculatedColumnFormula>COUNTIF(T_p4p3p2[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="stack" dataDxfId="195">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0A00-000002000000}" name="stack" dataDxfId="180">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,uncalled,IF(T_init[[#This Row],[p]]=2,sidepot2,IF(T_init[[#This Row],[p]]=3,sidepot1,IF(T_init[[#This Row],[p]]=4,mainpot,IF(ISBLANK(T_init[[#This Row],[p]]),T_init[[#This Row],[stack]],0)))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0A00-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="ICM" dataDxfId="194">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0A00-000004000000}" name="ICM" dataDxfId="179">
       <calculatedColumnFormula>T_p4p3p2[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="KO" dataDxfId="193">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0A00-000005000000}" name="KO" dataDxfId="178">
       <calculatedColumnFormula>T_p4p3p2[[#This Row],[players]]*T_p4p3p2[[#This Row],[stack]]/chips</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="$stack" dataDxfId="192">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0A00-000006000000}" name="$stack" dataDxfId="177">
       <calculatedColumnFormula>T_p4p3p2[[#This Row],[ICM]]+bounty*T_p4p3p2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4251,19 +4260,19 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="T_fact" displayName="T_fact" ref="BJ15:BO21" totalsRowShown="0" tableBorderDxfId="191">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF0B000000}" name="T_fact" displayName="T_fact" ref="BJ15:BO21" totalsRowShown="0" tableBorderDxfId="176">
   <autoFilter ref="BJ15:BO21" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0B00-000001000000}" name="players"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0B00-000002000000}" name="stack"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0B00-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="ICM" dataDxfId="190">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0B00-000004000000}" name="ICM" dataDxfId="175">
       <calculatedColumnFormula>T_fact[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="KO" dataDxfId="189">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0B00-000005000000}" name="KO" dataDxfId="174">
       <calculatedColumnFormula>IF(OR(T_init[[#This Row],[p]]=1, T_init[[#This Row],[p]]=3),T_fact[[#This Row],[players]]*T_fact[[#This Row],[stack]]/chips+1,T_fact[[#This Row],[players]]*T_fact[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="$stack" dataDxfId="188">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0B00-000006000000}" name="$stack" dataDxfId="173">
       <calculatedColumnFormula>T_fact[[#This Row],[ICM]]+bounty*T_fact[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4272,19 +4281,19 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="T_EV_p3sp2" displayName="T_EV_p3sp2" ref="BQ15:BT21" totalsRowShown="0" tableBorderDxfId="187">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{00000000-000C-0000-FFFF-FFFF0C000000}" name="T_EV_p3sp2" displayName="T_EV_p3sp2" ref="BQ15:BT21" totalsRowShown="0" tableBorderDxfId="172">
   <autoFilter ref="BQ15:BT21" xr:uid="{00000000-0009-0000-0100-00000E000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="ICM" dataDxfId="186">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0C00-000001000000}" name="ICM" dataDxfId="171">
       <calculatedColumnFormula>p1sp2win*T_p3p1[[#This Row],[ICM]]+p2sp2win*T_p3p2[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="KO" dataDxfId="185">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0C00-000002000000}" name="KO" dataDxfId="170">
       <calculatedColumnFormula>bounty*(p1sp2win*T_p3p1[[#This Row],[KO]]+p2sp2win*T_p3p2[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="EV" dataDxfId="184">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0C00-000003000000}" name="EV" dataDxfId="169">
       <calculatedColumnFormula>T_EV_p3sp2[[#This Row],[ICM]]+T_EV_p3sp2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="chipEV" dataDxfId="183">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0C00-000004000000}" name="chipEV" dataDxfId="168">
       <calculatedColumnFormula>p1sp2win*T_p3p1[[#This Row],[stack]]+p2sp2win*T_p3p2[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4293,19 +4302,19 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="T_EV_p4p3sp2" displayName="T_EV_p4p3sp2" ref="BW15:BZ21" totalsRowShown="0" tableBorderDxfId="182">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{00000000-000C-0000-FFFF-FFFF0D000000}" name="T_EV_p4p3sp2" displayName="T_EV_p4p3sp2" ref="BW15:BZ21" totalsRowShown="0" tableBorderDxfId="167">
   <autoFilter ref="BW15:BZ21" xr:uid="{00000000-0009-0000-0100-00000F000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="ICM" dataDxfId="181">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0D00-000001000000}" name="ICM" dataDxfId="166">
       <calculatedColumnFormula>p1sp2win*T_p4p3p1[[#This Row],[ICM]]+p2sp2win*T_p4p3p2[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="KO" dataDxfId="180">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0D00-000002000000}" name="KO" dataDxfId="165">
       <calculatedColumnFormula>bounty*(p1sp2win*T_p4p3p1[[#This Row],[KO]]+p2sp2win*T_p4p3p2[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="EV" dataDxfId="179">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0D00-000003000000}" name="EV" dataDxfId="164">
       <calculatedColumnFormula>T_EV_p4p3sp2[[#This Row],[ICM]]+T_EV_p4p3sp2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="chipEV" dataDxfId="178">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0D00-000004000000}" name="chipEV" dataDxfId="163">
       <calculatedColumnFormula>p1sp2win*T_p4p3p1[[#This Row],[stack]]+p2sp2win*T_p4p3p2[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4314,19 +4323,19 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="T_EV_p4sp1" displayName="T_EV_p4sp1" ref="CC15:CF21" totalsRowShown="0" tableBorderDxfId="177">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{00000000-000C-0000-FFFF-FFFF0E000000}" name="T_EV_p4sp1" displayName="T_EV_p4sp1" ref="CC15:CF21" totalsRowShown="0" tableBorderDxfId="162">
   <autoFilter ref="CC15:CF21" xr:uid="{00000000-0009-0000-0100-000010000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="ICM" dataDxfId="176">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0E00-000001000000}" name="ICM" dataDxfId="161">
       <calculatedColumnFormula>p1sp1win*T_p4p1[[#This Row],[ICM]]+p2sp1win*T_p4p2[[#This Row],[ICM]]+p3sp1win*T_EV_p4p3sp2[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="KO" dataDxfId="175">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0E00-000002000000}" name="KO" dataDxfId="160">
       <calculatedColumnFormula>bounty*(p1sp1win*T_p4p1[[#This Row],[KO]]+p2sp1win*T_p4p2[[#This Row],[KO]])+p3sp1win*T_EV_p4p3sp2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="EV" dataDxfId="174">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0E00-000003000000}" name="EV" dataDxfId="159">
       <calculatedColumnFormula>T_EV_p4sp1[[#This Row],[ICM]]+T_EV_p4sp1[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="chipEV" dataDxfId="173">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0E00-000004000000}" name="chipEV" dataDxfId="158">
       <calculatedColumnFormula>p1sp1win*T_p4p1[[#This Row],[stack]]+p2sp1win*T_p4p2[[#This Row],[stack]]+p3sp1win*T_EV_p4p3sp2[[#This Row],[chipEV]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4335,28 +4344,28 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="T_EV" displayName="T_EV" ref="CI15:CN21" totalsRowShown="0" tableBorderDxfId="172">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{00000000-000C-0000-FFFF-FFFF0F000000}" name="T_EV" displayName="T_EV" ref="CI15:CN21" totalsRowShown="0" tableBorderDxfId="157">
   <autoFilter ref="CI15:CN21" xr:uid="{00000000-0009-0000-0100-000011000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="ICM" dataDxfId="171">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0F00-000001000000}" name="ICM" dataDxfId="156">
       <calculatedColumnFormula>p4win*(T_EV_p4sp1[[#This Row],[ICM]])+'4way'!p3win*T_EV_p3sp2[[#This Row],[ICM]]+'4way'!p2win*T_p2[[#This Row],[ICM]]+'4way'!p1win*T_p1[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="KO" dataDxfId="170">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0F00-000002000000}" name="KO" dataDxfId="155">
       <calculatedColumnFormula>p4win*(T_EV_p4sp1[[#This Row],[KO]])+'4way'!p3win*T_EV_p3sp2[[#This Row],[KO]]+bounty*('4way'!p2win*T_p2[[#This Row],[KO]]+'4way'!p1win*T_p1[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="EV" dataDxfId="169">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0F00-000003000000}" name="EV" dataDxfId="154">
       <calculatedColumnFormula>T_EV[[#This Row],[ICM]]+T_EV[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="chipEV" dataDxfId="168">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0F00-000004000000}" name="chipEV" dataDxfId="153">
       <calculatedColumnFormula>'4way'!p1win*T_p1[[#This Row],[stack]]+
 '4way'!p2win*T_p2[[#This Row],[stack]]+
 '4way'!p3win*(p1sp2win*T_p3p1[[#This Row],[stack]]+p2sp2win*T_p3p2[[#This Row],[stack]])+
 p4win*(p1sp1win*T_p4p1[[#This Row],[stack]]+p2sp1win*T_p4p2[[#This Row],[stack]]+p3sp1win*(p1sp2win*T_p4p3p1[[#This Row],[stack]]+p2sp2win*T_p4p3p2[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="cEVdiff" dataDxfId="167">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0F00-000005000000}" name="cEVdiff" dataDxfId="152">
       <calculatedColumnFormula>T_EV[[#This Row],[chipEV]]-T_fact[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="Evdiff" dataDxfId="166">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0F00-000006000000}" name="Evdiff" dataDxfId="151">
       <calculatedColumnFormula>T_EV[[#This Row],[EV]]-(T_fact[[#This Row],[ICM]]+bounty*T_fact[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4383,23 +4392,23 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="T_p12135" displayName="T_p12135" ref="F15:K21" totalsRowShown="0" tableBorderDxfId="165">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="34" xr:uid="{00000000-000C-0000-FFFF-FFFF11000000}" name="T_p12135" displayName="T_p12135" ref="F15:K21" totalsRowShown="0" tableBorderDxfId="150">
   <autoFilter ref="F15:K21" xr:uid="{00000000-0009-0000-0100-000022000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="players" dataDxfId="164">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1100-000001000000}" name="players" dataDxfId="149">
       <calculatedColumnFormula>COUNTIF(T_p12135[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="stack" dataDxfId="163">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1100-000002000000}" name="stack" dataDxfId="148">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,mainpot+sidepot1+sidepot2+uncalled,IF(T_init2034[[#This Row],[p]]&gt;1,0,T_init2034[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1100-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="ICM" dataDxfId="162">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1100-000004000000}" name="ICM" dataDxfId="147">
       <calculatedColumnFormula>T_p12135[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="KO" dataDxfId="161">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1100-000005000000}" name="KO" dataDxfId="146">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,T_p12135[[#This Row],[players]]*T_p12135[[#This Row],[stack]]/chips+COUNTIF(T_p12135[stack],0),T_p12135[[#This Row],[players]]*T_p12135[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="$stack" dataDxfId="160">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1100-000006000000}" name="$stack" dataDxfId="145">
       <calculatedColumnFormula>T_p12135[[#This Row],[ICM]]+bounty*T_p12135[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4408,23 +4417,23 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="T_p22236" displayName="T_p22236" ref="M15:R21" totalsRowShown="0" tableBorderDxfId="159">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="35" xr:uid="{00000000-000C-0000-FFFF-FFFF12000000}" name="T_p22236" displayName="T_p22236" ref="M15:R21" totalsRowShown="0" tableBorderDxfId="144">
   <autoFilter ref="M15:R21" xr:uid="{00000000-0009-0000-0100-000023000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="players" dataDxfId="158" totalsRowDxfId="157">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1200-000001000000}" name="players" dataDxfId="143" totalsRowDxfId="142">
       <calculatedColumnFormula>COUNTIF(T_p22236[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="stack" dataDxfId="156" totalsRowDxfId="155">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1200-000002000000}" name="stack" dataDxfId="141" totalsRowDxfId="140">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,uncalled,IF(T_init2034[[#This Row],[p]]=2,mainpot+sidepot1+sidepot2,IF(T_init2034[[#This Row],[p]]&gt;2,0,T_init2034[[#This Row],[stack]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="EQ" totalsRowDxfId="154"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="ICM" dataDxfId="153" totalsRowDxfId="152">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1200-000003000000}" name="EQ" totalsRowDxfId="139"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1200-000004000000}" name="ICM" dataDxfId="138" totalsRowDxfId="137">
       <calculatedColumnFormula>T_p22236[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="KO" dataDxfId="151" totalsRowDxfId="150">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1200-000005000000}" name="KO" dataDxfId="136" totalsRowDxfId="135">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=2,T_p22236[[#This Row],[players]]*T_p22236[[#This Row],[stack]]/chips+COUNTIF(T_p22236[stack],0),T_p22236[[#This Row],[players]]*T_p22236[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="$stack" dataDxfId="149">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1200-000006000000}" name="$stack" dataDxfId="134">
       <calculatedColumnFormula>T_p22236[[#This Row],[ICM]]+bounty*T_p22236[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4433,7 +4442,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:AK14" tableBorderDxfId="291">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A8:AK14" tableBorderDxfId="276">
   <autoFilter ref="A8:AK14" xr:uid="{00000000-0009-0000-0100-000001000000}">
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -4462,64 +4471,64 @@
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="hand"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="pWin"/>
     <tableColumn id="30" xr3:uid="{00000000-0010-0000-0100-00001E000000}" name="players1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="stack1" dataDxfId="290" totalsRowDxfId="289"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="stack1" dataDxfId="275" totalsRowDxfId="274"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="EQ1"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="ICM1" dataDxfId="288">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="ICM1" dataDxfId="273">
       <calculatedColumnFormula>Table1[[#This Row],[EQ1]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="KO1" dataDxfId="287"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="players2" dataDxfId="286"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="stack2" dataDxfId="285" totalsRowDxfId="284"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="KO1" dataDxfId="272"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0100-00001F000000}" name="players2" dataDxfId="271"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="stack2" dataDxfId="270" totalsRowDxfId="269"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="EQ2"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ICM2" dataDxfId="283">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="ICM2" dataDxfId="268">
       <calculatedColumnFormula>Table1[[#This Row],[EQ2]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="KO2" dataDxfId="282" totalsRowDxfId="281">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="KO2" dataDxfId="267" totalsRowDxfId="266">
       <calculatedColumnFormula>5*Table2[[#This Row],[stacklose]]/3000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="KO22" dataDxfId="280"/>
-    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="playersside1" dataDxfId="279" totalsRowDxfId="278"/>
-    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="stackside1" dataDxfId="277"/>
-    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="EQside1" dataDxfId="276"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="ICMside1" dataDxfId="275">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0100-000020000000}" name="KO22" dataDxfId="265"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0100-000028000000}" name="playersside1" dataDxfId="264" totalsRowDxfId="263"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0100-000027000000}" name="stackside1" dataDxfId="262"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0100-000026000000}" name="EQside1" dataDxfId="261"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0100-000025000000}" name="ICMside1" dataDxfId="260">
       <calculatedColumnFormula>Table1[[#This Row],[EQside1]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="KOside1" dataDxfId="274" totalsRowDxfId="273">
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0100-000024000000}" name="KOside1" dataDxfId="259" totalsRowDxfId="258">
       <calculatedColumnFormula>Table1[[#This Row],[playersside1]]*Table1[[#This Row],[stackside1]]/3000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0100-000010000000}" name=" 2"/>
-    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0100-00002F000000}" name="playersside2" dataDxfId="272" totalsRowDxfId="271"/>
+    <tableColumn id="47" xr3:uid="{00000000-0010-0000-0100-00002F000000}" name="playersside2" dataDxfId="257" totalsRowDxfId="256"/>
     <tableColumn id="46" xr3:uid="{00000000-0010-0000-0100-00002E000000}" name="stackside2"/>
     <tableColumn id="45" xr3:uid="{00000000-0010-0000-0100-00002D000000}" name="EQside2"/>
-    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="ICMside2" dataDxfId="270">
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0100-00002C000000}" name="ICMside2" dataDxfId="255">
       <calculatedColumnFormula>Table1[[#This Row],[EQside2]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="KOside2" dataDxfId="269" totalsRowDxfId="268">
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0100-00002B000000}" name="KOside2" dataDxfId="254" totalsRowDxfId="253">
       <calculatedColumnFormula>Table1[[#This Row],[playersside2]]*Table1[[#This Row],[stackside2]]/3000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="42" xr3:uid="{00000000-0010-0000-0100-00002A000000}" name=" 3"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="playersf" dataDxfId="267" totalsRowDxfId="266"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="stackf" dataDxfId="265" totalsRowDxfId="264"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0100-000022000000}" name="playersf" dataDxfId="252" totalsRowDxfId="251"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0100-000011000000}" name="stackf" dataDxfId="250" totalsRowDxfId="249"/>
     <tableColumn id="18" xr3:uid="{00000000-0010-0000-0100-000012000000}" name="EQf"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="ICMf" dataDxfId="263">
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0100-000013000000}" name="ICMf" dataDxfId="248">
       <calculatedColumnFormula>Table1[[#This Row],[EQf]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KOf" dataDxfId="262" totalsRowDxfId="261">
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0100-000014000000}" name="KOf" dataDxfId="247" totalsRowDxfId="246">
       <calculatedColumnFormula>Table1[[#This Row],[playersf]]*Table1[[#This Row],[stackf]]/3000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="eqdiff" dataDxfId="260">
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0100-000015000000}" name="eqdiff" dataDxfId="245">
       <calculatedColumnFormula>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="ICMd" dataDxfId="259" totalsRowDxfId="258">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0100-000016000000}" name="ICMd" dataDxfId="244" totalsRowDxfId="243">
       <calculatedColumnFormula>p1win*Table1[[#This Row],[ICM1]]+(1-p1win)*(p2win*Table1[[#This Row],[ICM2]]+(1-p2win)*(p1spwin*Table1[[#This Row],[ICMside1]]+(1-p1spwin)*Table1[[#This Row],[ICMside2]])) -Table1[[#This Row],[ICMf]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="KOd" dataDxfId="257">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0100-000017000000}" name="KOd" dataDxfId="242">
       <calculatedColumnFormula>p3win*(p1spwin*Table1[[#This Row],[KOside1]]+(1-p1spwin)*Table1[[#This Row],[KOside2]])+p2win*Table1[[#This Row],[KO2]]+p1win*Table1[[#This Row],[KO1]] -Table1[[#This Row],[KOf]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="totald" totalsRowFunction="sum" dataDxfId="256">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0100-000019000000}" name="totald" totalsRowFunction="sum" dataDxfId="241">
       <calculatedColumnFormula>Table1[[#This Row],[ICMd]]+Table1[[#This Row],[KOd]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="cEVdiff" dataDxfId="255">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0100-00000C000000}" name="cEVdiff" dataDxfId="240">
       <calculatedColumnFormula>p3win*(p1spwin*Table1[[#This Row],[stackside1]]+(1-p1spwin)*Table1[[#This Row],[stackside2]])+p2win*Table1[[#This Row],[stack2]]+p1win*Table1[[#This Row],[stack1]] -Table1[[#This Row],[stackf]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4528,23 +4537,23 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="T_p3p12337" displayName="T_p3p12337" ref="T15:Y21" totalsRowShown="0" tableBorderDxfId="148">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="36" xr:uid="{00000000-000C-0000-FFFF-FFFF13000000}" name="T_p3p12337" displayName="T_p3p12337" ref="T15:Y21" totalsRowShown="0" tableBorderDxfId="133">
   <autoFilter ref="T15:Y21" xr:uid="{00000000-0009-0000-0100-000024000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="players" dataDxfId="147">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1300-000001000000}" name="players" dataDxfId="132">
       <calculatedColumnFormula>COUNTIF(T_p3p12337[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="stack" dataDxfId="146">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1300-000002000000}" name="stack" dataDxfId="131">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,sidepot1+uncalled,IF(T_init2034[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init2034[[#This Row],[p]]),T_init2034[[#This Row],[stack]],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1300-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="ICM" dataDxfId="145">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1300-000004000000}" name="ICM" dataDxfId="130">
       <calculatedColumnFormula>T_p3p12337[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="KO" dataDxfId="144">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1300-000005000000}" name="KO" dataDxfId="129">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,T_p3p12337[[#This Row],[players]]*T_p3p12337[[#This Row],[stack]]/chips+COUNTIF(T_p3p12337[stack],0),T_p3p12337[[#This Row],[players]]*T_p3p12337[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1300-000006000000}" name="$stack" dataDxfId="143">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1300-000006000000}" name="$stack" dataDxfId="128">
       <calculatedColumnFormula>T_p3p12337[[#This Row],[ICM]]+bounty*T_p3p12337[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4553,23 +4562,23 @@
 </file>
 
 <file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="T_p3p22438" displayName="T_p3p22438" ref="AA15:AF21" totalsRowShown="0" tableBorderDxfId="142">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="37" xr:uid="{00000000-000C-0000-FFFF-FFFF14000000}" name="T_p3p22438" displayName="T_p3p22438" ref="AA15:AF21" totalsRowShown="0" tableBorderDxfId="127">
   <autoFilter ref="AA15:AF21" xr:uid="{00000000-0009-0000-0100-000025000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="players" dataDxfId="141" totalsRowDxfId="140">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1400-000001000000}" name="players" dataDxfId="126" totalsRowDxfId="125">
       <calculatedColumnFormula>COUNTIF(T_p3p22438[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="stack" dataDxfId="139" totalsRowDxfId="138">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1400-000002000000}" name="stack" dataDxfId="124" totalsRowDxfId="123">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,uncalled,IF(T_init2034[[#This Row],[p]]=2,sidepot1,IF(T_init2034[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init2034[[#This Row],[p]]),T_init2034[[#This Row],[stack]],0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="EQ" totalsRowDxfId="137"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="ICM" dataDxfId="136" totalsRowDxfId="135">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1400-000003000000}" name="EQ" totalsRowDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1400-000004000000}" name="ICM" dataDxfId="121" totalsRowDxfId="120">
       <calculatedColumnFormula>T_p3p22438[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="KO" dataDxfId="134" totalsRowDxfId="133">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1400-000005000000}" name="KO" dataDxfId="119" totalsRowDxfId="118">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=2,T_p3p22438[[#This Row],[players]]*T_p3p22438[[#This Row],[stack]]/chips+COUNTIF(T_p3p22438[stack],0),T_p3p22438[[#This Row],[players]]*T_p3p22438[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="$stack" dataDxfId="132">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1400-000006000000}" name="$stack" dataDxfId="117">
       <calculatedColumnFormula>T_p3p22438[[#This Row],[ICM]]+bounty*T_p3p22438[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4578,23 +4587,23 @@
 </file>
 
 <file path=xl/tables/table22.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="T_fact2939" displayName="T_fact2939" ref="AI15:AN21" totalsRowShown="0" tableBorderDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="38" xr:uid="{00000000-000C-0000-FFFF-FFFF15000000}" name="T_fact2939" displayName="T_fact2939" ref="AI15:AN21" totalsRowShown="0" tableBorderDxfId="116">
   <autoFilter ref="AI15:AN21" xr:uid="{00000000-0009-0000-0100-000026000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1500-000001000000}" name="players">
       <calculatedColumnFormula>COUNTIF(T_fact2939[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="stack" dataDxfId="130">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1500-000002000000}" name="stack" dataDxfId="115">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,mainpot+sidepot1+sidepot2+uncalled,IF(T_init2034[[#This Row],[p]]&gt;1,0,T_init2034[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1500-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="ICM" dataDxfId="129">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1500-000004000000}" name="ICM" dataDxfId="114">
       <calculatedColumnFormula>T_fact2939[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="KO" dataDxfId="128">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1500-000005000000}" name="KO" dataDxfId="113">
       <calculatedColumnFormula>IF(T_init2034[[#This Row],[p]]=1,T_fact2939[[#This Row],[players]]*T_fact2939[[#This Row],[stack]]/chips+COUNTIF(T_fact2939[stack],0),T_fact2939[[#This Row],[players]]*T_fact2939[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="$stack" dataDxfId="127">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1500-000006000000}" name="$stack" dataDxfId="112">
       <calculatedColumnFormula>T_fact2939[[#This Row],[ICM]]+bounty*T_fact2939[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4603,33 +4612,33 @@
 </file>
 
 <file path=xl/tables/table23.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="T_EV3340" displayName="T_EV3340" ref="AQ15:AV21" totalsRowShown="0" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="39" xr:uid="{00000000-000C-0000-FFFF-FFFF16000000}" name="T_EV3340" displayName="T_EV3340" ref="AQ15:AV21" totalsRowShown="0" tableBorderDxfId="111">
   <autoFilter ref="AQ15:AV21" xr:uid="{00000000-0009-0000-0100-000027000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="ICM" dataDxfId="125">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1600-000001000000}" name="ICM" dataDxfId="110">
       <calculatedColumnFormula>'3wKhQs'!p3win* ('3wKhQs'!p1sp1win*T_p3p12337[[#This Row],[ICM]] + '3wKhQs'!p2sp1win*T_p3p22438[[#This Row],[ICM]])
 +'3wKhQs'!p2win*T_p22236[[#This Row],[ICM]]
 +'3wKhQs'!p1win*T_p12135[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="KO" dataDxfId="124">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1600-000002000000}" name="KO" dataDxfId="109">
       <calculatedColumnFormula>('3wKhQs'!p3win* ('3wKhQs'!p1sp1win*T_p3p12337[[#This Row],[KO]] + '3wKhQs'!p2sp1win*T_p3p22438[[#This Row],[KO]])
 +'3wKhQs'!p2win*T_p22236[[#This Row],[KO]]
 +'3wKhQs'!p1win*T_p12135[[#This Row],[KO]])*bounty</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="EV" dataDxfId="123">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1600-000003000000}" name="EV" dataDxfId="108">
       <calculatedColumnFormula>'3wKhQs'!p3win* ('3wKhQs'!p1sp1win*T_p3p12337[[#This Row],[$stack]] + '3wKhQs'!p2sp1win*T_p3p22438[[#This Row],[$stack]])
 +'3wKhQs'!p2win*T_p22236[[#This Row],[$stack]]
 +'3wKhQs'!p1win*T_p12135[[#This Row],[$stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="chipEV" dataDxfId="122">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1600-000004000000}" name="chipEV" dataDxfId="107">
       <calculatedColumnFormula>'3wKhQs'!p3win* ('3wKhQs'!p1sp1win*T_p3p12337[[#This Row],[stack]] + '3wKhQs'!p2sp1win*T_p3p22438[[#This Row],[stack]])
 +'3wKhQs'!p2win*T_p22236[[#This Row],[stack]]
 +'3wKhQs'!p1win*T_p12135[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1600-000005000000}" name="cEVdiff" dataDxfId="121">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1600-000005000000}" name="cEVdiff" dataDxfId="106">
       <calculatedColumnFormula>T_EV3340[[#This Row],[chipEV]]-T_fact2939[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1600-000006000000}" name="Evdiff" dataDxfId="120">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1600-000006000000}" name="Evdiff" dataDxfId="105">
       <calculatedColumnFormula>T_EV3340[[#This Row],[EV]]-(T_fact2939[[#This Row],[ICM]]+bounty*T_fact2939[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4656,23 +4665,23 @@
 </file>
 
 <file path=xl/tables/table25.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="T_p121" displayName="T_p121" ref="F15:K21" totalsRowShown="0" tableBorderDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{00000000-000C-0000-FFFF-FFFF18000000}" name="T_p121" displayName="T_p121" ref="F15:K21" totalsRowShown="0" tableBorderDxfId="104">
   <autoFilter ref="F15:K21" xr:uid="{00000000-0009-0000-0100-000014000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="players" dataDxfId="118">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1800-000001000000}" name="players" dataDxfId="103">
       <calculatedColumnFormula>COUNTIF(T_p121[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="stack" dataDxfId="117">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1800-000002000000}" name="stack" dataDxfId="102">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,mainpot+sidepot1+sidepot2+uncalled,IF(T_init20[[#This Row],[p]]&gt;1,0,T_init20[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1800-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="ICM" dataDxfId="116">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1800-000004000000}" name="ICM" dataDxfId="101">
       <calculatedColumnFormula>T_p121[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="KO" dataDxfId="115">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1800-000005000000}" name="KO" dataDxfId="100">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,T_p121[[#This Row],[players]]*T_p121[[#This Row],[stack]]/chips+COUNTIF(T_p121[stack],0),T_p121[[#This Row],[players]]*T_p121[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1800-000006000000}" name="$stack" dataDxfId="114">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1800-000006000000}" name="$stack" dataDxfId="99">
       <calculatedColumnFormula>T_p121[[#This Row],[ICM]]+bounty*T_p121[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4681,23 +4690,23 @@
 </file>
 
 <file path=xl/tables/table26.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="T_p222" displayName="T_p222" ref="M15:R21" totalsRowShown="0" tableBorderDxfId="113">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{00000000-000C-0000-FFFF-FFFF19000000}" name="T_p222" displayName="T_p222" ref="M15:R21" totalsRowShown="0" tableBorderDxfId="98">
   <autoFilter ref="M15:R21" xr:uid="{00000000-0009-0000-0100-000015000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="players" dataDxfId="112" totalsRowDxfId="111">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1900-000001000000}" name="players" dataDxfId="97" totalsRowDxfId="96">
       <calculatedColumnFormula>COUNTIF(T_p222[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="stack" dataDxfId="110" totalsRowDxfId="109">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1900-000002000000}" name="stack" dataDxfId="95" totalsRowDxfId="94">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,uncalled,IF(T_init20[[#This Row],[p]]=2,mainpot+sidepot1+sidepot2,IF(T_init20[[#This Row],[p]]&gt;2,0,T_init20[[#This Row],[stack]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1900-000003000000}" name="EQ" totalsRowDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="ICM" dataDxfId="107" totalsRowDxfId="106">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1900-000003000000}" name="EQ" totalsRowDxfId="93"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1900-000004000000}" name="ICM" dataDxfId="92" totalsRowDxfId="91">
       <calculatedColumnFormula>T_p222[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1900-000005000000}" name="KO" dataDxfId="105" totalsRowDxfId="104">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1900-000005000000}" name="KO" dataDxfId="90" totalsRowDxfId="89">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=2,T_p222[[#This Row],[players]]*T_p222[[#This Row],[stack]]/chips+COUNTIF(T_p222[stack],0),T_p222[[#This Row],[players]]*T_p222[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1900-000006000000}" name="$stack" dataDxfId="103">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1900-000006000000}" name="$stack" dataDxfId="88">
       <calculatedColumnFormula>T_p222[[#This Row],[ICM]]+bounty*T_p222[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4706,23 +4715,23 @@
 </file>
 
 <file path=xl/tables/table27.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="T_p3p123" displayName="T_p3p123" ref="T15:Y21" totalsRowShown="0" tableBorderDxfId="102">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="22" xr:uid="{00000000-000C-0000-FFFF-FFFF1A000000}" name="T_p3p123" displayName="T_p3p123" ref="T15:Y21" totalsRowShown="0" tableBorderDxfId="87">
   <autoFilter ref="T15:Y21" xr:uid="{00000000-0009-0000-0100-000016000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="players" dataDxfId="101">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1A00-000001000000}" name="players" dataDxfId="86">
       <calculatedColumnFormula>COUNTIF(T_p3p123[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="stack" dataDxfId="100">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1A00-000002000000}" name="stack" dataDxfId="85">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,sidepot1+uncalled,IF(T_init20[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init20[[#This Row],[p]]),T_init20[[#This Row],[stack]],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1A00-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1A00-000004000000}" name="ICM" dataDxfId="99">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1A00-000004000000}" name="ICM" dataDxfId="84">
       <calculatedColumnFormula>T_p3p123[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1A00-000005000000}" name="KO" dataDxfId="98">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1A00-000005000000}" name="KO" dataDxfId="83">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,T_p3p123[[#This Row],[players]]*T_p3p123[[#This Row],[stack]]/chips+COUNTIF(T_p3p123[stack],0),T_p3p123[[#This Row],[players]]*T_p3p123[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1A00-000006000000}" name="$stack" dataDxfId="97">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1A00-000006000000}" name="$stack" dataDxfId="82">
       <calculatedColumnFormula>T_p3p123[[#This Row],[ICM]]+bounty*T_p3p123[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4731,23 +4740,23 @@
 </file>
 
 <file path=xl/tables/table28.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="T_p3p224" displayName="T_p3p224" ref="AA15:AF21" totalsRowShown="0" tableBorderDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="23" xr:uid="{00000000-000C-0000-FFFF-FFFF1B000000}" name="T_p3p224" displayName="T_p3p224" ref="AA15:AF21" totalsRowShown="0" tableBorderDxfId="81">
   <autoFilter ref="AA15:AF21" xr:uid="{00000000-0009-0000-0100-000017000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="players" dataDxfId="95" totalsRowDxfId="94">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1B00-000001000000}" name="players" dataDxfId="80" totalsRowDxfId="79">
       <calculatedColumnFormula>COUNTIF(T_p3p224[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1B00-000002000000}" name="stack" dataDxfId="93" totalsRowDxfId="92">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1B00-000002000000}" name="stack" dataDxfId="78" totalsRowDxfId="77">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,uncalled,IF(T_init20[[#This Row],[p]]=2,sidepot1,IF(T_init20[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init20[[#This Row],[p]]),T_init20[[#This Row],[stack]],0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1B00-000003000000}" name="EQ" totalsRowDxfId="91"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1B00-000004000000}" name="ICM" dataDxfId="90" totalsRowDxfId="89">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1B00-000003000000}" name="EQ" totalsRowDxfId="76"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1B00-000004000000}" name="ICM" dataDxfId="75" totalsRowDxfId="74">
       <calculatedColumnFormula>T_p3p224[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1B00-000005000000}" name="KO" dataDxfId="88" totalsRowDxfId="87">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1B00-000005000000}" name="KO" dataDxfId="73" totalsRowDxfId="72">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=2,T_p3p224[[#This Row],[players]]*T_p3p224[[#This Row],[stack]]/chips+COUNTIF(T_p3p224[stack],0),T_p3p224[[#This Row],[players]]*T_p3p224[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1B00-000006000000}" name="$stack" dataDxfId="86">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1B00-000006000000}" name="$stack" dataDxfId="71">
       <calculatedColumnFormula>T_p3p224[[#This Row],[ICM]]+bounty*T_p3p224[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4756,23 +4765,23 @@
 </file>
 
 <file path=xl/tables/table29.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="T_fact29" displayName="T_fact29" ref="AI15:AN21" totalsRowShown="0" tableBorderDxfId="85">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="28" xr:uid="{00000000-000C-0000-FFFF-FFFF1C000000}" name="T_fact29" displayName="T_fact29" ref="AI15:AN21" totalsRowShown="0" tableBorderDxfId="70">
   <autoFilter ref="AI15:AN21" xr:uid="{00000000-0009-0000-0100-00001C000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-1C00-000001000000}" name="players">
       <calculatedColumnFormula>COUNTIF(T_fact29[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1C00-000002000000}" name="stack" dataDxfId="84">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1C00-000002000000}" name="stack" dataDxfId="69">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,mainpot+sidepot1+sidepot2+uncalled,IF(T_init20[[#This Row],[p]]&gt;1,0,T_init20[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1C00-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1C00-000004000000}" name="ICM" dataDxfId="83">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1C00-000004000000}" name="ICM" dataDxfId="68">
       <calculatedColumnFormula>T_fact29[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1C00-000005000000}" name="KO" dataDxfId="82">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1C00-000005000000}" name="KO" dataDxfId="67">
       <calculatedColumnFormula>IF(T_init20[[#This Row],[p]]=1,T_fact29[[#This Row],[players]]*T_fact29[[#This Row],[stack]]/chips+COUNTIF(T_fact29[stack],0),T_fact29[[#This Row],[players]]*T_fact29[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1C00-000006000000}" name="$stack" dataDxfId="81">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1C00-000006000000}" name="$stack" dataDxfId="66">
       <calculatedColumnFormula>T_fact29[[#This Row],[ICM]]+bounty*T_fact29[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4799,33 +4808,33 @@
 </file>
 
 <file path=xl/tables/table30.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF1D000000}" name="T_EV33" displayName="T_EV33" ref="AQ15:AV21" totalsRowShown="0" tableBorderDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="32" xr:uid="{00000000-000C-0000-FFFF-FFFF1D000000}" name="T_EV33" displayName="T_EV33" ref="AQ15:AV21" totalsRowShown="0" tableBorderDxfId="65">
   <autoFilter ref="AQ15:AV21" xr:uid="{00000000-0009-0000-0100-000020000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="ICM" dataDxfId="79">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1D00-000001000000}" name="ICM" dataDxfId="64">
       <calculatedColumnFormula>'3wAdKd'!p3win* ('3wAdKd'!p1sp1win*T_p3p123[[#This Row],[ICM]] + '3wAdKd'!p2sp1win*T_p3p224[[#This Row],[ICM]])
 +'3wAdKd'!p2win*T_p222[[#This Row],[ICM]]
 +'3wAdKd'!p1win*T_p121[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1D00-000002000000}" name="KO" dataDxfId="78">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1D00-000002000000}" name="KO" dataDxfId="63">
       <calculatedColumnFormula>('3wAdKd'!p3win* ('3wAdKd'!p1sp1win*T_p3p123[[#This Row],[KO]] + '3wAdKd'!p2sp1win*T_p3p224[[#This Row],[KO]])
 +'3wAdKd'!p2win*T_p222[[#This Row],[KO]]
 +'3wAdKd'!p1win*T_p121[[#This Row],[KO]])*bounty</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1D00-000003000000}" name="EV" dataDxfId="77">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-1D00-000003000000}" name="EV" dataDxfId="62">
       <calculatedColumnFormula>'3wAdKd'!p3win* ('3wAdKd'!p1sp1win*T_p3p123[[#This Row],[$stack]] + '3wAdKd'!p2sp1win*T_p3p224[[#This Row],[$stack]])
 +'3wAdKd'!p2win*T_p222[[#This Row],[$stack]]
 +'3wAdKd'!p1win*T_p121[[#This Row],[$stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1D00-000004000000}" name="chipEV" dataDxfId="76">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1D00-000004000000}" name="chipEV" dataDxfId="61">
       <calculatedColumnFormula>'3wAdKd'!p3win* ('3wAdKd'!p1sp1win*T_p3p123[[#This Row],[stack]] + '3wAdKd'!p2sp1win*T_p3p224[[#This Row],[stack]])
 +'3wAdKd'!p2win*T_p222[[#This Row],[stack]]
 +'3wAdKd'!p1win*T_p121[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1D00-000005000000}" name="cEVdiff" dataDxfId="75">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1D00-000005000000}" name="cEVdiff" dataDxfId="60">
       <calculatedColumnFormula>T_EV33[[#This Row],[chipEV]]-T_fact29[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1D00-000006000000}" name="Evdiff" dataDxfId="74">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1D00-000006000000}" name="Evdiff" dataDxfId="59">
       <calculatedColumnFormula>T_EV33[[#This Row],[EV]]-(T_fact29[[#This Row],[ICM]]+bounty*T_fact29[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4852,23 +4861,23 @@
 </file>
 
 <file path=xl/tables/table32.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="T_p12142" displayName="T_p12142" ref="F15:K18" totalsRowShown="0" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="41" xr:uid="{00000000-000C-0000-FFFF-FFFF1F000000}" name="T_p12142" displayName="T_p12142" ref="F15:K18" totalsRowShown="0" tableBorderDxfId="58">
   <autoFilter ref="F15:K18" xr:uid="{00000000-0009-0000-0100-000029000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="players" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-1F00-000001000000}" name="players" dataDxfId="57">
       <calculatedColumnFormula>COUNTIF(T_p12142[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1F00-000002000000}" name="stack" dataDxfId="71">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-1F00-000002000000}" name="stack" dataDxfId="56">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,mainpot+sidepot1+sidepot2+uncalled,IF(T_init2041[[#This Row],[p]]&gt;1,0,T_init2041[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-1F00-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1F00-000004000000}" name="ICM" dataDxfId="70">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-1F00-000004000000}" name="ICM" dataDxfId="55">
       <calculatedColumnFormula>T_p12142[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1F00-000005000000}" name="KO" dataDxfId="69">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-1F00-000005000000}" name="KO" dataDxfId="54">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,T_p12142[[#This Row],[players]]*T_p12142[[#This Row],[stack]]/chips+COUNTIF(T_p12142[stack],0),T_p12142[[#This Row],[players]]*T_p12142[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1F00-000006000000}" name="$stack" dataDxfId="68">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-1F00-000006000000}" name="$stack" dataDxfId="53">
       <calculatedColumnFormula>T_p12142[[#This Row],[ICM]]+bounty*T_p12142[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4877,23 +4886,23 @@
 </file>
 
 <file path=xl/tables/table33.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{00000000-000C-0000-FFFF-FFFF20000000}" name="T_p22243" displayName="T_p22243" ref="M15:R18" totalsRowShown="0" tableBorderDxfId="67">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="42" xr:uid="{00000000-000C-0000-FFFF-FFFF20000000}" name="T_p22243" displayName="T_p22243" ref="M15:R18" totalsRowShown="0" tableBorderDxfId="52">
   <autoFilter ref="M15:R18" xr:uid="{00000000-0009-0000-0100-00002A000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2000-000001000000}" name="players" dataDxfId="66" totalsRowDxfId="65">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2000-000001000000}" name="players" dataDxfId="51" totalsRowDxfId="50">
       <calculatedColumnFormula>COUNTIF(T_p22243[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2000-000002000000}" name="stack" dataDxfId="64" totalsRowDxfId="63">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2000-000002000000}" name="stack" dataDxfId="49" totalsRowDxfId="48">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,uncalled,IF(T_init2041[[#This Row],[p]]=2,mainpot+sidepot1+sidepot2,IF(T_init2041[[#This Row],[p]]&gt;2,0,T_init2041[[#This Row],[stack]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2000-000003000000}" name="EQ" totalsRowDxfId="62"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2000-000004000000}" name="ICM" dataDxfId="61" totalsRowDxfId="60">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2000-000003000000}" name="EQ" totalsRowDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2000-000004000000}" name="ICM" dataDxfId="46" totalsRowDxfId="45">
       <calculatedColumnFormula>T_p22243[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2000-000005000000}" name="KO" dataDxfId="59" totalsRowDxfId="58">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2000-000005000000}" name="KO" dataDxfId="44" totalsRowDxfId="43">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=2,T_p22243[[#This Row],[players]]*T_p22243[[#This Row],[stack]]/chips+COUNTIF(T_p22243[stack],0),T_p22243[[#This Row],[players]]*T_p22243[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2000-000006000000}" name="$stack" dataDxfId="57">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2000-000006000000}" name="$stack" dataDxfId="42">
       <calculatedColumnFormula>T_p22243[[#This Row],[ICM]]+bounty*T_p22243[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4902,23 +4911,23 @@
 </file>
 
 <file path=xl/tables/table34.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{00000000-000C-0000-FFFF-FFFF21000000}" name="T_p3p12344" displayName="T_p3p12344" ref="T15:Y18" totalsRowShown="0" tableBorderDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="43" xr:uid="{00000000-000C-0000-FFFF-FFFF21000000}" name="T_p3p12344" displayName="T_p3p12344" ref="T15:Y18" totalsRowShown="0" tableBorderDxfId="41">
   <autoFilter ref="T15:Y18" xr:uid="{00000000-0009-0000-0100-00002B000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2100-000001000000}" name="players" dataDxfId="55">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2100-000001000000}" name="players" dataDxfId="40">
       <calculatedColumnFormula>COUNTIF(T_p3p12344[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2100-000002000000}" name="stack" dataDxfId="54">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2100-000002000000}" name="stack" dataDxfId="39">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,sidepot1+uncalled,IF(T_init2041[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init2041[[#This Row],[p]]),T_init2041[[#This Row],[stack]],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-2100-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2100-000004000000}" name="ICM" dataDxfId="53">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2100-000004000000}" name="ICM" dataDxfId="38">
       <calculatedColumnFormula>T_p3p12344[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2100-000005000000}" name="KO" dataDxfId="52">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2100-000005000000}" name="KO" dataDxfId="37">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,T_p3p12344[[#This Row],[players]]*T_p3p12344[[#This Row],[stack]]/chips+COUNTIF(T_p3p12344[stack],0),T_p3p12344[[#This Row],[players]]*T_p3p12344[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2100-000006000000}" name="$stack" dataDxfId="51">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2100-000006000000}" name="$stack" dataDxfId="36">
       <calculatedColumnFormula>T_p3p12344[[#This Row],[ICM]]+bounty*T_p3p12344[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4927,23 +4936,23 @@
 </file>
 
 <file path=xl/tables/table35.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{00000000-000C-0000-FFFF-FFFF22000000}" name="T_p3p22445" displayName="T_p3p22445" ref="AA15:AF18" totalsRowShown="0" tableBorderDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="44" xr:uid="{00000000-000C-0000-FFFF-FFFF22000000}" name="T_p3p22445" displayName="T_p3p22445" ref="AA15:AF18" totalsRowShown="0" tableBorderDxfId="35">
   <autoFilter ref="AA15:AF18" xr:uid="{00000000-0009-0000-0100-00002C000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2200-000001000000}" name="players" dataDxfId="49" totalsRowDxfId="48">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2200-000001000000}" name="players" dataDxfId="34" totalsRowDxfId="33">
       <calculatedColumnFormula>COUNTIF(T_p3p22445[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2200-000002000000}" name="stack" dataDxfId="47" totalsRowDxfId="46">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2200-000002000000}" name="stack" dataDxfId="32" totalsRowDxfId="31">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,uncalled,IF(T_init2041[[#This Row],[p]]=2,sidepot1,IF(T_init2041[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init2041[[#This Row],[p]]),T_init2041[[#This Row],[stack]],0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2200-000003000000}" name="EQ" totalsRowDxfId="45"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2200-000004000000}" name="ICM" dataDxfId="44" totalsRowDxfId="43">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2200-000003000000}" name="EQ" totalsRowDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2200-000004000000}" name="ICM" dataDxfId="29" totalsRowDxfId="28">
       <calculatedColumnFormula>T_p3p22445[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2200-000005000000}" name="KO" dataDxfId="42" totalsRowDxfId="41">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2200-000005000000}" name="KO" dataDxfId="27" totalsRowDxfId="26">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=2,T_p3p22445[[#This Row],[players]]*T_p3p22445[[#This Row],[stack]]/chips+COUNTIF(T_p3p22445[stack],0),T_p3p22445[[#This Row],[players]]*T_p3p22445[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2200-000006000000}" name="$stack" dataDxfId="40">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2200-000006000000}" name="$stack" dataDxfId="25">
       <calculatedColumnFormula>T_p3p22445[[#This Row],[ICM]]+bounty*T_p3p22445[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4952,23 +4961,23 @@
 </file>
 
 <file path=xl/tables/table36.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{00000000-000C-0000-FFFF-FFFF23000000}" name="T_fact2946" displayName="T_fact2946" ref="AI15:AN18" totalsRowShown="0" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="45" xr:uid="{00000000-000C-0000-FFFF-FFFF23000000}" name="T_fact2946" displayName="T_fact2946" ref="AI15:AN18" totalsRowShown="0" tableBorderDxfId="24">
   <autoFilter ref="AI15:AN18" xr:uid="{00000000-0009-0000-0100-00002D000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-2300-000001000000}" name="players">
       <calculatedColumnFormula>COUNTIF(T_fact2946[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2300-000002000000}" name="stack" dataDxfId="38">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2300-000002000000}" name="stack" dataDxfId="23">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,sidepot1+uncalled,IF(T_init2041[[#This Row],[p]]=3,mainpot,IF(ISBLANK(T_init2041[[#This Row],[p]]),T_init2041[[#This Row],[stack]],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-2300-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2300-000004000000}" name="ICM" dataDxfId="37">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2300-000004000000}" name="ICM" dataDxfId="22">
       <calculatedColumnFormula>T_fact2946[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2300-000005000000}" name="KO" dataDxfId="36">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2300-000005000000}" name="KO" dataDxfId="21">
       <calculatedColumnFormula>IF(T_init2041[[#This Row],[p]]=1,T_fact2946[[#This Row],[players]]*T_fact2946[[#This Row],[stack]]/chips+COUNTIF(T_fact2946[stack],0),T_fact2946[[#This Row],[players]]*T_fact2946[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2300-000006000000}" name="$stack" dataDxfId="35">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2300-000006000000}" name="$stack" dataDxfId="20">
       <calculatedColumnFormula>T_fact2946[[#This Row],[ICM]]+bounty*T_fact2946[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4977,33 +4986,33 @@
 </file>
 
 <file path=xl/tables/table37.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{00000000-000C-0000-FFFF-FFFF24000000}" name="T_EV3347" displayName="T_EV3347" ref="AQ15:AV18" totalsRowShown="0" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="46" xr:uid="{00000000-000C-0000-FFFF-FFFF24000000}" name="T_EV3347" displayName="T_EV3347" ref="AQ15:AV18" totalsRowShown="0" tableBorderDxfId="19">
   <autoFilter ref="AQ15:AV18" xr:uid="{00000000-0009-0000-0100-00002E000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2400-000001000000}" name="ICM" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-2400-000001000000}" name="ICM" dataDxfId="18">
       <calculatedColumnFormula>'3wAh9s'!p3win* ('3wAh9s'!p1sp1win*T_p3p12344[[#This Row],[ICM]] + '3wAh9s'!p2sp1win*T_p3p22445[[#This Row],[ICM]])
 +'3wAh9s'!p2win*T_p22243[[#This Row],[ICM]]
 +'3wAh9s'!p1win*T_p12142[[#This Row],[ICM]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2400-000002000000}" name="KO" dataDxfId="32">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-2400-000002000000}" name="KO" dataDxfId="17">
       <calculatedColumnFormula>('3wAh9s'!p3win* ('3wAh9s'!p1sp1win*T_p3p12344[[#This Row],[KO]] + '3wAh9s'!p2sp1win*T_p3p22445[[#This Row],[KO]])
 +'3wAh9s'!p2win*T_p22243[[#This Row],[KO]]
 +'3wAh9s'!p1win*T_p12142[[#This Row],[KO]])*bounty</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2400-000003000000}" name="EV" dataDxfId="31">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-2400-000003000000}" name="EV" dataDxfId="16">
       <calculatedColumnFormula>'3wAh9s'!p3win* ('3wAh9s'!p1sp1win*T_p3p12344[[#This Row],[$stack]] + '3wAh9s'!p2sp1win*T_p3p22445[[#This Row],[$stack]])
 +'3wAh9s'!p2win*T_p22243[[#This Row],[$stack]]
 +'3wAh9s'!p1win*T_p12142[[#This Row],[$stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2400-000004000000}" name="chipEV" dataDxfId="30">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-2400-000004000000}" name="chipEV" dataDxfId="15">
       <calculatedColumnFormula>'3wAh9s'!p3win* ('3wAh9s'!p1sp1win*T_p3p12344[[#This Row],[stack]] + '3wAh9s'!p2sp1win*T_p3p22445[[#This Row],[stack]])
 +'3wAh9s'!p2win*T_p22243[[#This Row],[stack]]
 +'3wAh9s'!p1win*T_p12142[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2400-000005000000}" name="cEVdiff" dataDxfId="29">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-2400-000005000000}" name="cEVdiff" dataDxfId="14">
       <calculatedColumnFormula>T_EV3347[[#This Row],[chipEV]]-T_fact2946[[#This Row],[stack]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2400-000006000000}" name="Evdiff" dataDxfId="28">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-2400-000006000000}" name="Evdiff" dataDxfId="13">
       <calculatedColumnFormula>T_EV3347[[#This Row],[EV]]-(T_fact2946[[#This Row],[ICM]]+bounty*T_fact2946[[#This Row],[KO]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5012,23 +5021,23 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="T_p1" displayName="T_p1" ref="F15:K21" totalsRowShown="0" tableBorderDxfId="254">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="T_p1" displayName="T_p1" ref="F15:K21" totalsRowShown="0" tableBorderDxfId="239">
   <autoFilter ref="F15:K21" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="players" dataDxfId="253">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="players" dataDxfId="238">
       <calculatedColumnFormula>COUNTIF(T_p1[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="stack" dataDxfId="252">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="stack" dataDxfId="237">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,mainpot+sidepot1+sidepot2+uncalled,IF(T_init[[#This Row],[p]]&gt;1,0,T_init[[#This Row],[stack]]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ICM" dataDxfId="251">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="ICM" dataDxfId="236">
       <calculatedColumnFormula>T_p1[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="KO" dataDxfId="250">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="KO" dataDxfId="235">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,T_p1[[#This Row],[players]]*T_p1[[#This Row],[stack]]/chips+COUNTIF(T_p1[stack],0),T_p1[[#This Row],[players]]*T_p1[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="$stack" dataDxfId="249">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0300-000006000000}" name="$stack" dataDxfId="234">
       <calculatedColumnFormula>T_p1[[#This Row],[ICM]]+bounty*T_p1[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5037,23 +5046,23 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="T_p2" displayName="T_p2" ref="M15:R21" totalsRowShown="0" tableBorderDxfId="248">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="T_p2" displayName="T_p2" ref="M15:R21" totalsRowShown="0" tableBorderDxfId="233">
   <autoFilter ref="M15:R21" xr:uid="{00000000-0009-0000-0100-000006000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="players" dataDxfId="247" totalsRowDxfId="246">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="players" dataDxfId="232" totalsRowDxfId="231">
       <calculatedColumnFormula>COUNTIF(T_p2[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="stack" dataDxfId="245" totalsRowDxfId="244">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="stack" dataDxfId="230" totalsRowDxfId="229">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,uncalled,IF(T_init[[#This Row],[p]]=2,mainpot+sidepot1+sidepot2,IF(T_init[[#This Row],[p]]&gt;2,0,T_init[[#This Row],[stack]])))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="EQ" totalsRowDxfId="243"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ICM" dataDxfId="242" totalsRowDxfId="241">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="EQ" totalsRowDxfId="228"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="ICM" dataDxfId="227" totalsRowDxfId="226">
       <calculatedColumnFormula>T_p2[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="KO" dataDxfId="240" totalsRowDxfId="239">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="KO" dataDxfId="225" totalsRowDxfId="224">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=2,T_p2[[#This Row],[players]]*T_p2[[#This Row],[stack]]/chips+COUNTIF(T_p2[stack],0),T_p2[[#This Row],[players]]*T_p2[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="$stack" dataDxfId="238">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0400-000006000000}" name="$stack" dataDxfId="223">
       <calculatedColumnFormula>T_p2[[#This Row],[ICM]]+bounty*T_p2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5062,23 +5071,23 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="T_p3p1" displayName="T_p3p1" ref="T15:Y21" totalsRowShown="0" tableBorderDxfId="237">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="T_p3p1" displayName="T_p3p1" ref="T15:Y21" totalsRowShown="0" tableBorderDxfId="222">
   <autoFilter ref="T15:Y21" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="players" dataDxfId="236">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="players" dataDxfId="221">
       <calculatedColumnFormula>COUNTIF(T_p3p1[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="stack" dataDxfId="235">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="stack" dataDxfId="220">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,sidepot2+uncalled,IF(T_init[[#This Row],[p]]=3,mainpot+sidepot1,IF(ISBLANK(T_init[[#This Row],[p]]),T_init[[#This Row],[stack]],0)))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="ICM" dataDxfId="234">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="ICM" dataDxfId="219">
       <calculatedColumnFormula>T_p3p1[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="KO" dataDxfId="233">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="KO" dataDxfId="218">
       <calculatedColumnFormula>IF(OR(T_init[[#This Row],[p]]=1, T_init[[#This Row],[p]]=3),T_p3p1[[#This Row],[players]]*T_p3p1[[#This Row],[stack]]/chips+1,T_p3p1[[#This Row],[players]]*T_p3p1[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="$stack" dataDxfId="232">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="$stack" dataDxfId="217">
       <calculatedColumnFormula>T_p3p1[[#This Row],[ICM]]+bounty*T_p3p1[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5087,23 +5096,23 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="T_p3p2" displayName="T_p3p2" ref="AA15:AF21" totalsRowShown="0" tableBorderDxfId="231">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="T_p3p2" displayName="T_p3p2" ref="AA15:AF21" totalsRowShown="0" tableBorderDxfId="216">
   <autoFilter ref="AA15:AF21" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="players" dataDxfId="230" totalsRowDxfId="229">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="players" dataDxfId="215" totalsRowDxfId="214">
       <calculatedColumnFormula>COUNTIF(T_p3p2[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="stack" dataDxfId="228" totalsRowDxfId="227">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="stack" dataDxfId="213" totalsRowDxfId="212">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,uncalled,IF(T_init[[#This Row],[p]]=2,sidepot2,IF(T_init[[#This Row],[p]]=3,mainpot+sidepot1,IF(ISBLANK(T_init[[#This Row],[p]]),T_init[[#This Row],[stack]],0))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="EQ" totalsRowDxfId="226"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="ICM" dataDxfId="225" totalsRowDxfId="224">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="EQ" totalsRowDxfId="211"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="ICM" dataDxfId="210" totalsRowDxfId="209">
       <calculatedColumnFormula>T_p3p2[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="KO" dataDxfId="223" totalsRowDxfId="222">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="KO" dataDxfId="208" totalsRowDxfId="207">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=3,T_p3p2[[#This Row],[players]]*T_p3p2[[#This Row],[stack]]/chips+1,T_p3p2[[#This Row],[players]]*T_p3p2[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="$stack" dataDxfId="221">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="$stack" dataDxfId="206">
       <calculatedColumnFormula>T_p3p2[[#This Row],[ICM]]+bounty*T_p3p2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5112,23 +5121,23 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="T_p4p1" displayName="T_p4p1" ref="AH15:AM21" totalsRowShown="0" tableBorderDxfId="220">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="T_p4p1" displayName="T_p4p1" ref="AH15:AM21" totalsRowShown="0" tableBorderDxfId="205">
   <autoFilter ref="AH15:AM21" xr:uid="{00000000-0009-0000-0100-000009000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="players" dataDxfId="219" totalsRowDxfId="218">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="players" dataDxfId="204" totalsRowDxfId="203">
       <calculatedColumnFormula>COUNTIF(T_p4p1[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="stack" dataDxfId="217" totalsRowDxfId="216">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="stack" dataDxfId="202" totalsRowDxfId="201">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=4,mainpot,IF(T_init[[#This Row],[p]]=1,sidepot1+sidepot2+uncalled,IF(ISBLANK(T_init[[#This Row],[p]]),T_init[[#This Row],[stack]],0)))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="EQ" totalsRowDxfId="215"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="ICM" dataDxfId="214" totalsRowDxfId="213">
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="EQ" totalsRowDxfId="200"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="ICM" dataDxfId="199" totalsRowDxfId="198">
       <calculatedColumnFormula>T_p4p1[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="KO" dataDxfId="212" totalsRowDxfId="211">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="KO" dataDxfId="197" totalsRowDxfId="196">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,T_p4p1[[#This Row],[players]]*T_p4p1[[#This Row],[stack]]/chips+2,T_p4p1[[#This Row],[players]]*T_p4p1[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="$stack" dataDxfId="210">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="$stack" dataDxfId="195">
       <calculatedColumnFormula>T_p4p1[[#This Row],[ICM]]+bounty*T_p4p1[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5137,23 +5146,23 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="T_p4p2" displayName="T_p4p2" ref="AO15:AT21" totalsRowShown="0" tableBorderDxfId="209">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{00000000-000C-0000-FFFF-FFFF08000000}" name="T_p4p2" displayName="T_p4p2" ref="AO15:AT21" totalsRowShown="0" tableBorderDxfId="194">
   <autoFilter ref="AO15:AT21" xr:uid="{00000000-0009-0000-0100-00000A000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="players" dataDxfId="208">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0800-000001000000}" name="players" dataDxfId="193">
       <calculatedColumnFormula>COUNTIF(T_p4p2[stack],"&gt;0")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="stack" dataDxfId="207">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0800-000002000000}" name="stack" dataDxfId="192">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=1,uncalled,IF(T_init[[#This Row],[p]]=2,sidepot1+sidepot2,IF(T_init[[#This Row],[p]]=4,mainpot,IF(ISBLANK(T_init[[#This Row],[p]]),T_init[[#This Row],[stack]],0))))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0800-000003000000}" name="EQ"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="ICM" dataDxfId="206">
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0800-000004000000}" name="ICM" dataDxfId="191">
       <calculatedColumnFormula>T_p4p2[[#This Row],[EQ]]*prize</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="KO" dataDxfId="205">
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0800-000005000000}" name="KO" dataDxfId="190">
       <calculatedColumnFormula>IF(T_init[[#This Row],[p]]=2,T_p4p2[[#This Row],[players]]*T_p4p2[[#This Row],[stack]]/chips+1,T_p4p2[[#This Row],[players]]*T_p4p2[[#This Row],[stack]]/chips)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="$stack" dataDxfId="204">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0800-000006000000}" name="$stack" dataDxfId="189">
       <calculatedColumnFormula>T_p4p2[[#This Row],[ICM]]+bounty*T_p4p2[[#This Row],[KO]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5427,7 +5436,7 @@
   <dimension ref="A1:X1048505"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="X61" sqref="X61"/>
+      <selection activeCell="X69" sqref="X69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9023,7 +9032,7 @@
       </c>
       <c r="H56" s="43"/>
       <c r="J56" s="41">
-        <f>I56*$E$1</f>
+        <f t="shared" ref="J56:J86" si="10">I56*$E$1</f>
         <v>0</v>
       </c>
       <c r="K56" s="44">
@@ -9032,7 +9041,7 @@
       </c>
       <c r="M56" s="45"/>
       <c r="O56" s="41">
-        <f>N56*$E$1</f>
+        <f t="shared" ref="O56:O86" si="11">N56*$E$1</f>
         <v>0</v>
       </c>
       <c r="P56" s="46">
@@ -9097,7 +9106,7 @@
         <v>0.71</v>
       </c>
       <c r="J57" s="2">
-        <f>I57*$E$1</f>
+        <f t="shared" si="10"/>
         <v>193.12</v>
       </c>
       <c r="K57" s="14">
@@ -9111,7 +9120,7 @@
         <v>0</v>
       </c>
       <c r="O57" s="2">
-        <f>N57*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P57" s="15">
@@ -9176,7 +9185,7 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="J58" s="18">
-        <f>I58*$E$1</f>
+        <f t="shared" si="10"/>
         <v>78.88</v>
       </c>
       <c r="K58" s="20">
@@ -9190,7 +9199,7 @@
         <v>1</v>
       </c>
       <c r="O58" s="18">
-        <f>N58*$E$1</f>
+        <f t="shared" si="11"/>
         <v>272</v>
       </c>
       <c r="P58" s="22">
@@ -9237,7 +9246,7 @@
       </c>
       <c r="H59" s="43"/>
       <c r="J59" s="41">
-        <f>I59*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K59" s="44">
@@ -9246,7 +9255,7 @@
       </c>
       <c r="M59" s="45"/>
       <c r="O59" s="41">
-        <f>N59*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P59" s="46">
@@ -9311,7 +9320,7 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="J60" s="2">
-        <f>I60*$E$1</f>
+        <f t="shared" si="10"/>
         <v>76.160000000000011</v>
       </c>
       <c r="K60" s="14">
@@ -9325,7 +9334,7 @@
         <v>0</v>
       </c>
       <c r="O60" s="2">
-        <f>N60*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P60" s="15">
@@ -9392,7 +9401,7 @@
         <v>0.45</v>
       </c>
       <c r="J61" s="18">
-        <f>I61*$E$1</f>
+        <f t="shared" si="10"/>
         <v>122.4</v>
       </c>
       <c r="K61" s="20">
@@ -9408,7 +9417,7 @@
         <v>0.73</v>
       </c>
       <c r="O61" s="18">
-        <f>N61*$E$1</f>
+        <f t="shared" si="11"/>
         <v>198.56</v>
       </c>
       <c r="P61" s="22">
@@ -9473,7 +9482,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="J62" s="2">
-        <f>I62*$E$1</f>
+        <f t="shared" si="10"/>
         <v>61.2</v>
       </c>
       <c r="K62" s="14">
@@ -9488,7 +9497,7 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="O62" s="2">
-        <f>N62*$E$1</f>
+        <f t="shared" si="11"/>
         <v>61.2</v>
       </c>
       <c r="P62" s="15">
@@ -9550,7 +9559,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="J63" s="2">
-        <f>I63*$E$1</f>
+        <f t="shared" si="10"/>
         <v>12.24</v>
       </c>
       <c r="K63" s="14">
@@ -9565,7 +9574,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O63" s="2">
-        <f>N63*$E$1</f>
+        <f t="shared" si="11"/>
         <v>12.24</v>
       </c>
       <c r="P63" s="15">
@@ -9609,7 +9618,7 @@
       </c>
       <c r="H64" s="43"/>
       <c r="J64" s="41">
-        <f>I64*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K64" s="44">
@@ -9618,7 +9627,7 @@
       </c>
       <c r="M64" s="45"/>
       <c r="O64" s="41">
-        <f>N64*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P64" s="46">
@@ -9650,45 +9659,69 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D65" s="10"/>
+    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>595</v>
+      </c>
+      <c r="B65" t="s">
+        <v>200</v>
+      </c>
+      <c r="C65">
+        <v>0.27950000000000003</v>
+      </c>
+      <c r="D65" s="10">
+        <v>570</v>
+      </c>
+      <c r="E65">
+        <v>0.28499999999999998</v>
+      </c>
       <c r="F65" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
-        <v>0</v>
+        <v>77.52</v>
       </c>
       <c r="G65" s="16">
         <f>2*Table2[[#This Row],[stackwin]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="H65" s="10"/>
+        <v>0.38</v>
+      </c>
+      <c r="H65" s="10">
+        <v>640</v>
+      </c>
+      <c r="I65">
+        <v>0.32</v>
+      </c>
       <c r="J65" s="2">
-        <f>I65*$E$1</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>87.04</v>
       </c>
       <c r="K65" s="14">
         <f>5*Table2[[#This Row],[stacklose]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="M65" s="8"/>
+        <v>1.0666666666666667</v>
+      </c>
+      <c r="M65" s="10">
+        <v>640</v>
+      </c>
+      <c r="N65">
+        <v>0.32</v>
+      </c>
       <c r="O65" s="2">
-        <f>N65*$E$1</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>87.04</v>
       </c>
       <c r="P65" s="15">
         <f>5*Table2[[#This Row],[stackfact]]/3000</f>
-        <v>0</v>
+        <v>1.0666666666666667</v>
       </c>
       <c r="Q65" s="38">
         <f>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</f>
-        <v>0</v>
+        <v>-9.7825000000000273E-3</v>
       </c>
       <c r="R65" s="12">
         <f>Table2[[#This Row],[pWin]]*Table2[[#This Row],[ICMwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[ICMlose]]-Table2[[#This Row],[ICMFact]]</f>
-        <v>0</v>
+        <v>-2.6608400000000074</v>
       </c>
       <c r="S65" s="16">
         <f>Table2[[#This Row],[Kowin]]*Table2[[#This Row],[pWin]]+Table2[[#This Row],[Kolose]]*(1-Table2[[#This Row],[pWin]])-Table2[[#This Row],[KOFact]]</f>
-        <v>0</v>
+        <v>-0.19192333333333333</v>
       </c>
       <c r="T65" s="2">
         <f>Table2[[#This Row],[KODiff]]*bounty</f>
@@ -9696,40 +9729,61 @@
       </c>
       <c r="U65" s="7">
         <f>Table2[[#This Row],[ICMdiff]]+Table2[[#This Row],[KOmoneyDiff]]</f>
-        <v>0</v>
+        <v>-2.6608400000000074</v>
       </c>
       <c r="V65" s="38">
         <f>Table2[[#This Row],[pWin]]*Table2[[#This Row],[stackwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[stacklose]]-Table2[[#This Row],[stackfact]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D66" s="10"/>
+        <v>-19.565000000000055</v>
+      </c>
+    </row>
+    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>975</v>
+      </c>
+      <c r="C66">
+        <v>0.27950000000000003</v>
+      </c>
+      <c r="D66" s="10">
+        <v>965</v>
+      </c>
+      <c r="E66">
+        <v>0.48249999999999998</v>
+      </c>
       <c r="F66" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
-        <v>0</v>
+        <v>131.24</v>
       </c>
       <c r="G66" s="16">
         <f>2*Table2[[#This Row],[stackwin]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="H66" s="10"/>
+        <v>0.64333333333333331</v>
+      </c>
+      <c r="H66" s="10">
+        <v>965</v>
+      </c>
+      <c r="I66">
+        <v>0.48249999999999998</v>
+      </c>
       <c r="J66" s="2">
-        <f>I66*$E$1</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>131.24</v>
       </c>
       <c r="K66" s="14">
         <f>5*Table2[[#This Row],[stacklose]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="M66" s="8"/>
+        <v>1.6083333333333334</v>
+      </c>
+      <c r="M66" s="10">
+        <v>965</v>
+      </c>
+      <c r="N66">
+        <v>0.48249999999999998</v>
+      </c>
       <c r="O66" s="2">
-        <f>N66*$E$1</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>131.24</v>
       </c>
       <c r="P66" s="15">
         <f>5*Table2[[#This Row],[stackfact]]/3000</f>
-        <v>0</v>
+        <v>1.6083333333333334</v>
       </c>
       <c r="Q66" s="38">
         <f>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</f>
@@ -9741,7 +9795,7 @@
       </c>
       <c r="S66" s="16">
         <f>Table2[[#This Row],[Kowin]]*Table2[[#This Row],[pWin]]+Table2[[#This Row],[Kolose]]*(1-Table2[[#This Row],[pWin]])-Table2[[#This Row],[KOFact]]</f>
-        <v>0</v>
+        <v>-0.26971750000000005</v>
       </c>
       <c r="T66" s="2">
         <f>Table2[[#This Row],[KODiff]]*bounty</f>
@@ -9756,33 +9810,54 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D67" s="10"/>
+    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>405</v>
+      </c>
+      <c r="C67">
+        <v>0.27950000000000003</v>
+      </c>
+      <c r="D67" s="10">
+        <v>395</v>
+      </c>
+      <c r="E67">
+        <v>0.19750000000000001</v>
+      </c>
       <c r="F67" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
-        <v>0</v>
+        <v>53.72</v>
       </c>
       <c r="G67" s="16">
         <f>2*Table2[[#This Row],[stackwin]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="10"/>
+        <v>0.26333333333333331</v>
+      </c>
+      <c r="H67" s="10">
+        <v>395</v>
+      </c>
+      <c r="I67">
+        <v>0.19750000000000001</v>
+      </c>
       <c r="J67" s="2">
-        <f>I67*$E$1</f>
-        <v>0</v>
+        <f t="shared" si="10"/>
+        <v>53.72</v>
       </c>
       <c r="K67" s="14">
         <f>5*Table2[[#This Row],[stacklose]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="M67" s="8"/>
+        <v>0.65833333333333333</v>
+      </c>
+      <c r="M67" s="10">
+        <v>395</v>
+      </c>
+      <c r="N67">
+        <v>0.19750000000000001</v>
+      </c>
       <c r="O67" s="2">
-        <f>N67*$E$1</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>53.72</v>
       </c>
       <c r="P67" s="15">
         <f>5*Table2[[#This Row],[stackfact]]/3000</f>
-        <v>0</v>
+        <v>0.65833333333333333</v>
       </c>
       <c r="Q67" s="38">
         <f>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</f>
@@ -9794,7 +9869,7 @@
       </c>
       <c r="S67" s="16">
         <f>Table2[[#This Row],[Kowin]]*Table2[[#This Row],[pWin]]+Table2[[#This Row],[Kolose]]*(1-Table2[[#This Row],[pWin]])-Table2[[#This Row],[KOFact]]</f>
-        <v>0</v>
+        <v>-0.11040250000000007</v>
       </c>
       <c r="T67" s="2">
         <f>Table2[[#This Row],[KODiff]]*bounty</f>
@@ -9809,113 +9884,140 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D68" s="10"/>
-      <c r="F68" s="2">
+    <row r="68" spans="1:24" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="17">
+        <v>25</v>
+      </c>
+      <c r="B68" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C68" s="17">
+        <v>0.27950000000000003</v>
+      </c>
+      <c r="D68" s="19">
+        <v>70</v>
+      </c>
+      <c r="E68" s="17">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="F68" s="18">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
-        <v>0</v>
-      </c>
-      <c r="G68" s="16">
+        <v>9.5200000000000014</v>
+      </c>
+      <c r="G68" s="24">
         <f>2*Table2[[#This Row],[stackwin]]/3000</f>
-        <v>0</v>
-      </c>
-      <c r="H68" s="10"/>
-      <c r="J68" s="2">
-        <f>I68*$E$1</f>
-        <v>0</v>
-      </c>
-      <c r="K68" s="14">
+        <v>4.6666666666666669E-2</v>
+      </c>
+      <c r="H68" s="19">
+        <v>0</v>
+      </c>
+      <c r="I68" s="17">
+        <v>0</v>
+      </c>
+      <c r="J68" s="18">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K68" s="20">
         <f>5*Table2[[#This Row],[stacklose]]/3000</f>
         <v>0</v>
       </c>
-      <c r="M68" s="8"/>
-      <c r="O68" s="2">
-        <f>N68*$E$1</f>
-        <v>0</v>
-      </c>
-      <c r="P68" s="15">
+      <c r="M68" s="19">
+        <v>0</v>
+      </c>
+      <c r="N68" s="17">
+        <v>0</v>
+      </c>
+      <c r="O68" s="18">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P68" s="22">
         <f>5*Table2[[#This Row],[stackfact]]/3000</f>
         <v>0</v>
       </c>
-      <c r="Q68" s="38">
+      <c r="Q68" s="35">
         <f>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</f>
-        <v>0</v>
-      </c>
-      <c r="R68" s="12">
+        <v>9.7825000000000013E-3</v>
+      </c>
+      <c r="R68" s="23">
         <f>Table2[[#This Row],[pWin]]*Table2[[#This Row],[ICMwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[ICMlose]]-Table2[[#This Row],[ICMFact]]</f>
-        <v>0</v>
-      </c>
-      <c r="S68" s="16">
+        <v>2.6608400000000008</v>
+      </c>
+      <c r="S68" s="24">
         <f>Table2[[#This Row],[Kowin]]*Table2[[#This Row],[pWin]]+Table2[[#This Row],[Kolose]]*(1-Table2[[#This Row],[pWin]])-Table2[[#This Row],[KOFact]]</f>
-        <v>0</v>
-      </c>
-      <c r="T68" s="2">
+        <v>1.3043333333333336E-2</v>
+      </c>
+      <c r="T68" s="18">
         <f>Table2[[#This Row],[KODiff]]*bounty</f>
         <v>0</v>
       </c>
-      <c r="U68" s="7">
+      <c r="U68" s="25">
         <f>Table2[[#This Row],[ICMdiff]]+Table2[[#This Row],[KOmoneyDiff]]</f>
-        <v>0</v>
-      </c>
-      <c r="V68" s="38">
+        <v>2.6608400000000008</v>
+      </c>
+      <c r="V68" s="35">
         <f>Table2[[#This Row],[pWin]]*Table2[[#This Row],[stackwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[stacklose]]-Table2[[#This Row],[stackfact]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D69" s="10"/>
-      <c r="F69" s="2">
+        <v>19.565000000000001</v>
+      </c>
+      <c r="X68" s="17" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="69" spans="1:24" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D69" s="43"/>
+      <c r="F69" s="41">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
         <v>0</v>
       </c>
-      <c r="G69" s="16">
+      <c r="G69" s="42">
         <f>2*Table2[[#This Row],[stackwin]]/3000</f>
         <v>0</v>
       </c>
-      <c r="H69" s="10"/>
-      <c r="J69" s="2">
-        <f>I69*$E$1</f>
-        <v>0</v>
-      </c>
-      <c r="K69" s="14">
+      <c r="H69" s="43"/>
+      <c r="J69" s="41">
+        <f t="shared" si="10"/>
+        <v>0</v>
+      </c>
+      <c r="K69" s="44">
         <f>5*Table2[[#This Row],[stacklose]]/3000</f>
         <v>0</v>
       </c>
-      <c r="M69" s="8"/>
-      <c r="O69" s="2">
-        <f>N69*$E$1</f>
-        <v>0</v>
-      </c>
-      <c r="P69" s="15">
+      <c r="M69" s="45"/>
+      <c r="O69" s="41">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="P69" s="46">
         <f>5*Table2[[#This Row],[stackfact]]/3000</f>
         <v>0</v>
       </c>
-      <c r="Q69" s="38">
+      <c r="Q69" s="47">
         <f>Table2[[#This Row],[EQwin]]*Table2[[#This Row],[pWin]] + Table2[[#This Row],[EQlose]]*(1-Table2[[#This Row],[pWin]]) - Table2[[#This Row],[Eqfact]]</f>
         <v>0</v>
       </c>
-      <c r="R69" s="12">
+      <c r="R69" s="48">
         <f>Table2[[#This Row],[pWin]]*Table2[[#This Row],[ICMwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[ICMlose]]-Table2[[#This Row],[ICMFact]]</f>
         <v>0</v>
       </c>
-      <c r="S69" s="16">
+      <c r="S69" s="42">
         <f>Table2[[#This Row],[Kowin]]*Table2[[#This Row],[pWin]]+Table2[[#This Row],[Kolose]]*(1-Table2[[#This Row],[pWin]])-Table2[[#This Row],[KOFact]]</f>
         <v>0</v>
       </c>
-      <c r="T69" s="2">
+      <c r="T69" s="41">
         <f>Table2[[#This Row],[KODiff]]*bounty</f>
         <v>0</v>
       </c>
-      <c r="U69" s="7">
+      <c r="U69" s="49">
         <f>Table2[[#This Row],[ICMdiff]]+Table2[[#This Row],[KOmoneyDiff]]</f>
         <v>0</v>
       </c>
-      <c r="V69" s="38">
+      <c r="V69" s="47">
         <f>Table2[[#This Row],[pWin]]*Table2[[#This Row],[stackwin]]+(1-Table2[[#This Row],[pWin]])*Table2[[#This Row],[stacklose]]-Table2[[#This Row],[stackfact]]</f>
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D70" s="10"/>
       <c r="F70" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -9927,7 +10029,7 @@
       </c>
       <c r="H70" s="10"/>
       <c r="J70" s="2">
-        <f>I70*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K70" s="14">
@@ -9936,7 +10038,7 @@
       </c>
       <c r="M70" s="8"/>
       <c r="O70" s="2">
-        <f>N70*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P70" s="15">
@@ -9968,7 +10070,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D71" s="10"/>
       <c r="F71" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -9980,7 +10082,7 @@
       </c>
       <c r="H71" s="10"/>
       <c r="J71" s="2">
-        <f>I71*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K71" s="14">
@@ -9989,7 +10091,7 @@
       </c>
       <c r="M71" s="8"/>
       <c r="O71" s="2">
-        <f>N71*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P71" s="15">
@@ -10021,7 +10123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D72" s="10"/>
       <c r="F72" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10033,7 +10135,7 @@
       </c>
       <c r="H72" s="10"/>
       <c r="J72" s="2">
-        <f>I72*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K72" s="14">
@@ -10042,7 +10144,7 @@
       </c>
       <c r="M72" s="8"/>
       <c r="O72" s="2">
-        <f>N72*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P72" s="15">
@@ -10074,7 +10176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D73" s="10"/>
       <c r="F73" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10086,7 +10188,7 @@
       </c>
       <c r="H73" s="10"/>
       <c r="J73" s="2">
-        <f>I73*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K73" s="14">
@@ -10095,7 +10197,7 @@
       </c>
       <c r="M73" s="8"/>
       <c r="O73" s="2">
-        <f>N73*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P73" s="15">
@@ -10127,7 +10229,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D74" s="10"/>
       <c r="F74" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10139,7 +10241,7 @@
       </c>
       <c r="H74" s="10"/>
       <c r="J74" s="2">
-        <f>I74*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K74" s="14">
@@ -10148,7 +10250,7 @@
       </c>
       <c r="M74" s="8"/>
       <c r="O74" s="2">
-        <f>N74*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P74" s="15">
@@ -10180,7 +10282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D75" s="10"/>
       <c r="F75" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10192,7 +10294,7 @@
       </c>
       <c r="H75" s="10"/>
       <c r="J75" s="2">
-        <f>I75*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K75" s="14">
@@ -10201,7 +10303,7 @@
       </c>
       <c r="M75" s="8"/>
       <c r="O75" s="2">
-        <f>N75*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P75" s="15">
@@ -10233,7 +10335,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D76" s="10"/>
       <c r="F76" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10245,7 +10347,7 @@
       </c>
       <c r="H76" s="10"/>
       <c r="J76" s="2">
-        <f>I76*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K76" s="14">
@@ -10254,7 +10356,7 @@
       </c>
       <c r="M76" s="8"/>
       <c r="O76" s="2">
-        <f>N76*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P76" s="15">
@@ -10286,7 +10388,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D77" s="10"/>
       <c r="F77" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10298,7 +10400,7 @@
       </c>
       <c r="H77" s="10"/>
       <c r="J77" s="2">
-        <f>I77*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K77" s="14">
@@ -10307,7 +10409,7 @@
       </c>
       <c r="M77" s="8"/>
       <c r="O77" s="2">
-        <f>N77*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P77" s="15">
@@ -10339,7 +10441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D78" s="10"/>
       <c r="F78" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10351,7 +10453,7 @@
       </c>
       <c r="H78" s="10"/>
       <c r="J78" s="2">
-        <f>I78*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K78" s="14">
@@ -10360,7 +10462,7 @@
       </c>
       <c r="M78" s="8"/>
       <c r="O78" s="2">
-        <f>N78*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P78" s="15">
@@ -10392,7 +10494,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D79" s="10"/>
       <c r="F79" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10404,7 +10506,7 @@
       </c>
       <c r="H79" s="10"/>
       <c r="J79" s="2">
-        <f>I79*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K79" s="14">
@@ -10413,7 +10515,7 @@
       </c>
       <c r="M79" s="8"/>
       <c r="O79" s="2">
-        <f>N79*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P79" s="15">
@@ -10445,7 +10547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="4:22" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D80" s="10"/>
       <c r="F80" s="2">
         <f>Table2[[#This Row],[EQwin]]*$E$1</f>
@@ -10457,7 +10559,7 @@
       </c>
       <c r="H80" s="10"/>
       <c r="J80" s="2">
-        <f>I80*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K80" s="14">
@@ -10466,7 +10568,7 @@
       </c>
       <c r="M80" s="8"/>
       <c r="O80" s="2">
-        <f>N80*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P80" s="15">
@@ -10510,7 +10612,7 @@
       </c>
       <c r="H81" s="10"/>
       <c r="J81" s="2">
-        <f>I81*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K81" s="14">
@@ -10519,7 +10621,7 @@
       </c>
       <c r="M81" s="8"/>
       <c r="O81" s="2">
-        <f>N81*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P81" s="15">
@@ -10563,7 +10665,7 @@
       </c>
       <c r="H82" s="10"/>
       <c r="J82" s="2">
-        <f>I82*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K82" s="14">
@@ -10572,7 +10674,7 @@
       </c>
       <c r="M82" s="8"/>
       <c r="O82" s="2">
-        <f>N82*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P82" s="15">
@@ -10616,7 +10718,7 @@
       </c>
       <c r="H83" s="10"/>
       <c r="J83" s="2">
-        <f>I83*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K83" s="14">
@@ -10625,7 +10727,7 @@
       </c>
       <c r="M83" s="8"/>
       <c r="O83" s="2">
-        <f>N83*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P83" s="15">
@@ -10669,7 +10771,7 @@
       </c>
       <c r="H84" s="10"/>
       <c r="J84" s="2">
-        <f>I84*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K84" s="14">
@@ -10678,7 +10780,7 @@
       </c>
       <c r="M84" s="8"/>
       <c r="O84" s="2">
-        <f>N84*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P84" s="15">
@@ -10722,7 +10824,7 @@
       </c>
       <c r="H85" s="10"/>
       <c r="J85" s="2">
-        <f>I85*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K85" s="14">
@@ -10731,7 +10833,7 @@
       </c>
       <c r="M85" s="8"/>
       <c r="O85" s="2">
-        <f>N85*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P85" s="15">
@@ -10775,7 +10877,7 @@
       </c>
       <c r="H86" s="10"/>
       <c r="J86" s="2">
-        <f>I86*$E$1</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="K86" s="14">
@@ -10784,7 +10886,7 @@
       </c>
       <c r="M86" s="8"/>
       <c r="O86" s="2">
-        <f>N86*$E$1</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P86" s="15">
@@ -14796,6 +14898,19 @@
     </row>
   </sheetData>
   <mergeCells count="28">
+    <mergeCell ref="CI12:CL12"/>
+    <mergeCell ref="CI13:CL13"/>
+    <mergeCell ref="CI14:CL14"/>
+    <mergeCell ref="BJ14:BN14"/>
+    <mergeCell ref="BQ14:BT14"/>
+    <mergeCell ref="BQ12:BT12"/>
+    <mergeCell ref="BQ13:BT13"/>
+    <mergeCell ref="BW12:BZ12"/>
+    <mergeCell ref="BW13:BZ13"/>
+    <mergeCell ref="BW14:BZ14"/>
+    <mergeCell ref="CC12:CF12"/>
+    <mergeCell ref="CC13:CF13"/>
+    <mergeCell ref="CC14:CF14"/>
     <mergeCell ref="AH11:BG11"/>
     <mergeCell ref="AH12:BG12"/>
     <mergeCell ref="BW11:BZ11"/>
@@ -14811,19 +14926,6 @@
     <mergeCell ref="AO14:AS14"/>
     <mergeCell ref="AV14:AZ14"/>
     <mergeCell ref="AH13:AS13"/>
-    <mergeCell ref="CI12:CL12"/>
-    <mergeCell ref="CI13:CL13"/>
-    <mergeCell ref="CI14:CL14"/>
-    <mergeCell ref="BJ14:BN14"/>
-    <mergeCell ref="BQ14:BT14"/>
-    <mergeCell ref="BQ12:BT12"/>
-    <mergeCell ref="BQ13:BT13"/>
-    <mergeCell ref="BW12:BZ12"/>
-    <mergeCell ref="BW13:BZ13"/>
-    <mergeCell ref="BW14:BZ14"/>
-    <mergeCell ref="CC12:CF12"/>
-    <mergeCell ref="CC13:CF13"/>
-    <mergeCell ref="CC14:CF14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>